<commit_message>
creating new Translator For Sabio Class to seperate the Query Data Structures from Sabio String generation
</commit_message>
<xml_diff>
--- a/mypackage/Results From Mycoplasma_test.xlsx
+++ b/mypackage/Results From Mycoplasma_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -70,43 +70,97 @@
     <t>Closest Km Values</t>
   </si>
   <si>
-    <t>[c]: PI + INS &lt;==&gt; R1P + HYXN</t>
-  </si>
-  <si>
-    <t>125</t>
-  </si>
-  <si>
-    <t>0.00191666667</t>
-  </si>
-  <si>
-    <t>{'numParticipants': [2, 2], 'proximity': 7.0, 'km': u'1.0E-4', 'reactionID': u'125', 'entryID': u'48072', 'vmax': u'0.00191666667', 'reactionStoichiometry': u'Phosphate + Inosine = alpha-D-Ribose 1-phosphate + Hypoxanthine', 'species': u'Salmonella typhimurium', 'ECNumber': u'2.4.2.1'}</t>
-  </si>
-  <si>
-    <t>{'numParticipants': [2, 2], 'proximity': 7.0, 'km': u'1.2E-4', 'reactionID': u'125', 'entryID': u'48081', 'vmax': u'0.0011', 'reactionStoichiometry': u'Phosphate + Inosine = alpha-D-Ribose 1-phosphate + Hypoxanthine', 'species': u'Escherichia coli', 'ECNumber': u'2.4.2.1'}</t>
-  </si>
-  <si>
-    <t>{'numParticipants': [2, 2], 'proximity': 7.0, 'km': u'9.0E-5', 'reactionID': u'125', 'entryID': u'48073', 'vmax': u'0.00586666667', 'reactionStoichiometry': u'Phosphate + Inosine = alpha-D-Ribose 1-phosphate + Hypoxanthine', 'species': u'Salmonella typhimurium', 'ECNumber': u'2.4.2.1'}</t>
-  </si>
-  <si>
-    <t>7.0</t>
-  </si>
-  <si>
-    <t>Lift Not Used</t>
-  </si>
-  <si>
-    <t>48072, 48073, 48081, 48082</t>
-  </si>
-  <si>
-    <t>0.0011, 0.00191666667, 0.00383333333, 0.00586666667</t>
-  </si>
-  <si>
-    <t>9.0E-5</t>
-  </si>
-  <si>
-    <t>{'numParticipants': [2, 2], 'proximity': 7.0, 'km': u'7.0E-5', 'reactionID': u'125', 'entryID': u'48082', 'vmax': u'0.00383333333', 'reactionStoichiometry': u'Phosphate + Inosine = alpha-D-Ribose 1-phosphate + Hypoxanthine', 'species': u'Escherichia coli', 'ECNumber': u'2.4.2.1'}</t>
-  </si>
-  <si>
-    <t>1.0E-4, 1.2E-4, 7.0E-5, 9.0E-5</t>
+    <t>[c]: ATP + Pantetheine4Phosphate ==&gt; DPCOA + PPI</t>
+  </si>
+  <si>
+    <t>2884</t>
+  </si>
+  <si>
+    <t>0.00456666667</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': '', 'reactionID': u'201', 'entryID': u'17911', 'vmax': u'0.00456666667', 'reactionStoichiometry': u'ATP + UMP = UDP + ADP', 'species': u'Streptococcus pneumoniae', 'ECNumber': u'2.7.4.22'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'2.22E-5', 'reactionID': u'201', 'entryID': u'40434', 'vmax': u'5.33333333E-5', 'reactionStoichiometry': u'ATP + UMP = UDP + ADP', 'species': u'Streptococcus pneumoniae', 'ECNumber': u'2.7.4.22'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'30.0', 'reactionID': u'201', 'entryID': u'51897', 'vmax': u'25.0', 'reactionStoichiometry': u'ATP + UMP = UDP + ADP', 'species': u'Bacillus subtilis', 'ECNumber': u'2.7.4.22'}</t>
+  </si>
+  <si>
+    <t>6.0</t>
+  </si>
+  <si>
+    <t>Lifted From 2.7.4</t>
+  </si>
+  <si>
+    <t>11594, 11595, 11596, 17903, 17904, 17905, 17906, 17907, 17908, 17909, 17910, 17911, 17912, 17913, 17914, 17915, 17916, 17917, 17918, 17919, 17920, 17921, 17922, 17923, 17924, 17925, 17926, 17927, 17928, 17933, 17934, 17935, 40410, 40411, 40412, 40413, 40414, 40415, 40416, 40417, 40418, 40419, 40420, 40433, 40434, 40435, 40436, 49510, 51897, 51898, 51899</t>
+  </si>
+  <si>
+    <t>0.001155, 0.00126666667, 0.001335, 0.00225, 0.00303333333, 0.00375, 0.00456666667, 0.0048, 0.00665, 0.00966666667, 0.0111, 0.6, 24.0, 25.0, 3.03333333E-4, 3.8E-4, 4.6E-4, 4.91666667E-4, 5.33333333E-5, 5.66666667E-4, 6.36666667E-4, 6.43333333E-4, 6.96666667E-4, 8.66666667E-4, 8.83333333E-5, 9.85E-4</t>
+  </si>
+  <si>
+    <t>1.0E-4</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'1.0E-4', 'reactionID': u'201', 'entryID': u'17927', 'vmax': u'0.00665', 'reactionStoichiometry': u'ATP + UMP = UDP + ADP', 'species': u'Streptococcus pneumoniae', 'ECNumber': u'2.7.4.22'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'1.0E-5', 'reactionID': u'201', 'entryID': u'40435', 'vmax': u'8.83333333E-5', 'reactionStoichiometry': u'ATP + UMP = UDP + ADP', 'species': u'Bacillus subtilis', 'ECNumber': u'2.7.4.22'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'140.0', 'reactionID': u'13616', 'entryID': u'51899', 'vmax': u'0.6', 'reactionStoichiometry': u"ATP + 6-Azauridine 5'-phosphate = ADP + 6-Azauridine 5'-diphosphate", 'species': u'Bacillus subtilis', 'ECNumber': u'2.7.4.22'}</t>
+  </si>
+  <si>
+    <t>11594, 11595, 11596, 17927, 17928, 40415, 40418, 40419, 40420, 40433, 40434, 40435, 40436, 49510, 51897, 51898, 51899, 51903, 51904</t>
+  </si>
+  <si>
+    <t>0.9, 1.056E-4, 1.0E-4, 1.0E-5, 1.31E-4, 1.55E-4, 1.5E-4, 1.6E-5, 120.0, 140.0, 2.22E-5, 2.74E-5, 3.6E-5, 3.7E-5, 30.0, 7.6E-5, 8.0, 9.97E-5</t>
+  </si>
+  <si>
+    <t>[c]: e3dCMP + H2O ==&gt; e3dC + PI</t>
+  </si>
+  <si>
+    <t>4.33333333E-5</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'9.0E-6', 'reactionID': u'581', 'entryID': u'22920', 'vmax': u'4.33333333E-5', 'reactionStoichiometry': u'D-Mannitol 1-phosphate + H2O = Phosphate + D-Mannitol', 'species': u'Streptococcus bovis', 'ECNumber': u'3.1.3.22'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'0.07', 'reactionID': u'7713', 'entryID': u'22921', 'vmax': u'9.5E-6', 'reactionStoichiometry': u'H2O + Glucose 6-phosphate = Glucose + Phosphate', 'species': u'Streptococcus bovis', 'ECNumber': u'3.1.3.9'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 6.0, 'km': u'0.011', 'reactionID': u'2493', 'entryID': u'16039', 'vmax': u'3.5E-4', 'reactionStoichiometry': u'2-Deoxy-D-glucose 6-phosphate + H2O = 2-Deoxy-D-glucose + Phosphate', 'species': u'Lactococcus lactis subsp. lactis', 'ECNumber': u'3.1.3.2'}</t>
+  </si>
+  <si>
+    <t>Lifted From 3.1.3</t>
+  </si>
+  <si>
+    <t>16039, 16871, 16872, 22920, 22921, 22922, 42747</t>
+  </si>
+  <si>
+    <t>2.91666667E-5, 3.33333333E-5, 3.5E-4, 4.33333333E-5, 6.33333333E-5, 9.0E-5, 9.5E-6</t>
+  </si>
+  <si>
+    <t>2.6E-6</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 1.0, 'km': u'2.6E-6', 'reactionID': u'295', 'entryID': u'30219', 'vmax': u'', 'reactionStoichiometry': u'H2O + AMP = Phosphate + Adenosine', 'species': u'Mycoplasma fermentans', 'ECNumber': u'3.1.3.5'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 1.0, 'km': u'6.3E-7', 'reactionID': u'295', 'entryID': u'30226', 'vmax': u'', 'reactionStoichiometry': u'H2O + AMP = Phosphate + Adenosine', 'species': u'Mycoplasma pulmonis', 'ECNumber': u'3.1.3.5'}</t>
+  </si>
+  <si>
+    <t>{'numParticipants': [2, 2], 'proximity': 1.0, 'km': u'1.04E-5', 'reactionID': u'295', 'entryID': u'30224', 'vmax': u'', 'reactionStoichiometry': u'H2O + AMP = Phosphate + Adenosine', 'species': u'Mycoplasma fermentans', 'ECNumber': u'3.1.3.5'}</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>30218, 30219, 30220, 30221, 30222, 30223, 30224, 30225, 30226, 30227</t>
+  </si>
+  <si>
+    <t>1.04E-5, 1.0E-6, 1.8E-6, 2.2E-6, 2.6E-6, 4.1E-6, 4.2E-6, 6.3E-7</t>
   </si>
 </sst>
 </file>
@@ -443,7 +497,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -542,13 +596,13 @@
         <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
         <v>24</v>
@@ -557,10 +611,64 @@
         <v>25</v>
       </c>
       <c r="Q2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s"/>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>